<commit_message>
hotový import ip_manager v3.7 do trimazkonu
</commit_message>
<xml_diff>
--- a/Trideni_GUI_v2/saved_addresses_2.xlsx
+++ b/Trideni_GUI_v2/saved_addresses_2.xlsx
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -546,7 +546,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -604,31 +604,6 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>bewolktt</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>192.168.000.000</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>du hast einen problem</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -790,7 +765,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nova vizualizace pokrocileho nastaveni trimazkonu, potreba dodelat
</commit_message>
<xml_diff>
--- a/Trideni_GUI_v2/saved_addresses_2.xlsx
+++ b/Trideni_GUI_v2/saved_addresses_2.xlsx
@@ -745,7 +745,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -755,7 +755,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">

</xml_diff>